<commit_message>
update solar panel schematic
</commit_message>
<xml_diff>
--- a/Material/Inventory.xlsx
+++ b/Material/Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtolenti89\Documents\05_Electronics\Kicad\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F29AC03-DDEE-4238-B5C6-C039D15D426E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C48CFA-582B-4921-ACB6-6B5C94742213}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12825" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistor" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="IC" sheetId="8" r:id="rId8"/>
     <sheet name="Others" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="445">
   <si>
     <t>Part number</t>
   </si>
@@ -1478,6 +1478,21 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/100pcs-6-6-5mm-Light-touch-switch-DIP4-Touch-button-Touch-switch-6-6-5-keys/32866696732.html?spm=2114.search0104.3.1.5d9f4eb4dAjsi7&amp;ws_ab_test=searchweb0_0,searchweb201602_9_10065_10068_10547_319_317_10548_10696_10084_453_10083_454_10618_10304_10307_10820_10821_537_10302_536_10843_10059_10884_10887_321_322_10103,searchweb201603_51,ppcSwitch_0&amp;algo_expid=fbdfc942-55b2-4ec6-81b0-5b09b689e17d-0&amp;algo_pvid=fbdfc942-55b2-4ec6-81b0-5b09b689e17d&amp;transAbTest=ae803_3</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Rt</t>
+  </si>
+  <si>
+    <t>3.3/3.3</t>
+  </si>
+  <si>
+    <t>5.1k</t>
   </si>
 </sst>
 </file>
@@ -1874,8 +1889,8 @@
   <dimension ref="A1:AMK64"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,7 +2545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2547,7 +2562,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D34" s="1" t="s">
         <v>33</v>
       </c>
@@ -2564,7 +2579,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D35" s="1">
         <v>10</v>
       </c>
@@ -2581,7 +2596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D36" s="1">
         <v>22</v>
       </c>
@@ -2598,7 +2613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D37" s="1">
         <v>47</v>
       </c>
@@ -2615,7 +2630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D38" s="1">
         <v>62</v>
       </c>
@@ -2632,7 +2647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D39" s="1">
         <v>8</v>
       </c>
@@ -2649,7 +2664,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D40" s="1">
         <v>100</v>
       </c>
@@ -2666,7 +2681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D41" s="1">
         <v>150</v>
       </c>
@@ -2683,7 +2698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D42" s="1">
         <v>330</v>
       </c>
@@ -2700,7 +2715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D43" s="1">
         <v>470</v>
       </c>
@@ -2717,7 +2732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D44" s="1">
         <v>680</v>
       </c>
@@ -2734,7 +2749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D45" s="1" t="s">
         <v>12</v>
       </c>
@@ -2750,8 +2765,20 @@
       <c r="I45" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="K45" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="L45" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="46" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D46" s="1" t="s">
         <v>34</v>
       </c>
@@ -2767,8 +2794,20 @@
       <c r="I46" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="K46" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="L46" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="47" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D47" s="1" t="s">
         <v>15</v>
       </c>
@@ -2784,8 +2823,15 @@
       <c r="I47" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="K47" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="L47" s="1">
+        <f>L45*L46/(L45+L46)</f>
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="48" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D48" s="1" t="s">
         <v>16</v>
       </c>
@@ -3084,9 +3130,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4317,9 +4363,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
structure web watering software
</commit_message>
<xml_diff>
--- a/Material/Inventory.xlsx
+++ b/Material/Inventory.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtolenti89\Documents\05_Electronics\Kicad\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C48CFA-582B-4921-ACB6-6B5C94742213}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F3894-DDEF-4273-8B3B-BC0B189D4120}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12825" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistor" sheetId="1" r:id="rId1"/>
     <sheet name="Capacitor" sheetId="2" r:id="rId2"/>
     <sheet name="LED" sheetId="3" r:id="rId3"/>
-    <sheet name="Diode" sheetId="4" r:id="rId4"/>
-    <sheet name="Transistor" sheetId="5" r:id="rId5"/>
+    <sheet name="Transistor" sheetId="5" r:id="rId4"/>
+    <sheet name="Diode" sheetId="4" r:id="rId5"/>
     <sheet name="Voltage_Regulator" sheetId="6" r:id="rId6"/>
     <sheet name="Crystal" sheetId="7" r:id="rId7"/>
     <sheet name="IC" sheetId="8" r:id="rId8"/>
@@ -1499,7 +1499,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1511,6 +1511,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1537,7 +1544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1571,6 +1578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1889,8 +1897,8 @@
   <dimension ref="A1:AMK64"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,7 +2904,7 @@
         <v>31</v>
       </c>
       <c r="I51" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.25">
@@ -2930,7 +2938,7 @@
         <v>31</v>
       </c>
       <c r="I53" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.25">
@@ -3130,9 +3138,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4169,7 +4177,7 @@
   <dimension ref="A1:AMK6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4234,7 +4242,7 @@
         <v>1206</v>
       </c>
       <c r="I2" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4263,7 +4271,7 @@
         <v>1206</v>
       </c>
       <c r="I3" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4360,6 +4368,558 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:I68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A52" sqref="A52"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="6" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="1025" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>232</v>
+      </c>
+      <c r="B53" t="s">
+        <v>195</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E53" t="s">
+        <v>235</v>
+      </c>
+      <c r="G53" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53" t="s">
+        <v>236</v>
+      </c>
+      <c r="I53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>237</v>
+      </c>
+      <c r="B54" t="s">
+        <v>195</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E54" t="s">
+        <v>239</v>
+      </c>
+      <c r="G54" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54" t="s">
+        <v>236</v>
+      </c>
+      <c r="I54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>240</v>
+      </c>
+      <c r="B55" t="s">
+        <v>241</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E55" t="s">
+        <v>239</v>
+      </c>
+      <c r="F55" t="s">
+        <v>243</v>
+      </c>
+      <c r="G55" t="s">
+        <v>10</v>
+      </c>
+      <c r="H55" t="s">
+        <v>236</v>
+      </c>
+      <c r="I55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>244</v>
+      </c>
+      <c r="B56" t="s">
+        <v>245</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E56" t="s">
+        <v>239</v>
+      </c>
+      <c r="F56" t="s">
+        <v>247</v>
+      </c>
+      <c r="G56" t="s">
+        <v>10</v>
+      </c>
+      <c r="H56" t="s">
+        <v>236</v>
+      </c>
+      <c r="I56">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>248</v>
+      </c>
+      <c r="B57" t="s">
+        <v>249</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E57" t="s">
+        <v>235</v>
+      </c>
+      <c r="F57" t="s">
+        <v>251</v>
+      </c>
+      <c r="G57" t="s">
+        <v>10</v>
+      </c>
+      <c r="H57" t="s">
+        <v>236</v>
+      </c>
+      <c r="I57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>252</v>
+      </c>
+      <c r="B58" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E58" t="s">
+        <v>239</v>
+      </c>
+      <c r="F58" t="s">
+        <v>254</v>
+      </c>
+      <c r="G58" t="s">
+        <v>10</v>
+      </c>
+      <c r="H58" t="s">
+        <v>236</v>
+      </c>
+      <c r="I58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>255</v>
+      </c>
+      <c r="B59" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E59" t="s">
+        <v>235</v>
+      </c>
+      <c r="F59" t="s">
+        <v>254</v>
+      </c>
+      <c r="G59" t="s">
+        <v>10</v>
+      </c>
+      <c r="H59" t="s">
+        <v>236</v>
+      </c>
+      <c r="I59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>257</v>
+      </c>
+      <c r="B60" t="s">
+        <v>159</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E60" t="s">
+        <v>235</v>
+      </c>
+      <c r="F60" t="s">
+        <v>259</v>
+      </c>
+      <c r="G60" t="s">
+        <v>10</v>
+      </c>
+      <c r="H60" t="s">
+        <v>236</v>
+      </c>
+      <c r="I60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>260</v>
+      </c>
+      <c r="B61" t="s">
+        <v>159</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E61" t="s">
+        <v>239</v>
+      </c>
+      <c r="F61" t="s">
+        <v>259</v>
+      </c>
+      <c r="G61" t="s">
+        <v>10</v>
+      </c>
+      <c r="H61" t="s">
+        <v>236</v>
+      </c>
+      <c r="I61">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>262</v>
+      </c>
+      <c r="B62" t="s">
+        <v>159</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E62" t="s">
+        <v>239</v>
+      </c>
+      <c r="F62" t="s">
+        <v>264</v>
+      </c>
+      <c r="G62" t="s">
+        <v>10</v>
+      </c>
+      <c r="H62" t="s">
+        <v>236</v>
+      </c>
+      <c r="I62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>265</v>
+      </c>
+      <c r="B63" t="s">
+        <v>159</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E63" t="s">
+        <v>235</v>
+      </c>
+      <c r="F63" t="s">
+        <v>264</v>
+      </c>
+      <c r="G63" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63" t="s">
+        <v>236</v>
+      </c>
+      <c r="I63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>267</v>
+      </c>
+      <c r="B64" t="s">
+        <v>268</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E64" t="s">
+        <v>235</v>
+      </c>
+      <c r="F64" t="s">
+        <v>270</v>
+      </c>
+      <c r="G64" t="s">
+        <v>10</v>
+      </c>
+      <c r="H64" t="s">
+        <v>236</v>
+      </c>
+      <c r="I64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>271</v>
+      </c>
+      <c r="B65" t="s">
+        <v>272</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E65" t="s">
+        <v>239</v>
+      </c>
+      <c r="F65" t="s">
+        <v>274</v>
+      </c>
+      <c r="G65" t="s">
+        <v>10</v>
+      </c>
+      <c r="H65" t="s">
+        <v>236</v>
+      </c>
+      <c r="I65">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>13001</v>
+      </c>
+      <c r="B66" t="s">
+        <v>272</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E66" t="s">
+        <v>239</v>
+      </c>
+      <c r="F66" t="s">
+        <v>276</v>
+      </c>
+      <c r="G66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H66" t="s">
+        <v>236</v>
+      </c>
+      <c r="I66">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>430</v>
+      </c>
+      <c r="B67" t="s">
+        <v>431</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="E67" t="s">
+        <v>235</v>
+      </c>
+      <c r="F67" t="s">
+        <v>254</v>
+      </c>
+      <c r="G67" t="s">
+        <v>30</v>
+      </c>
+      <c r="H67" t="s">
+        <v>289</v>
+      </c>
+      <c r="I67">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>432</v>
+      </c>
+      <c r="B68" t="s">
+        <v>431</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="E68" t="s">
+        <v>239</v>
+      </c>
+      <c r="F68" t="s">
+        <v>254</v>
+      </c>
+      <c r="G68" t="s">
+        <v>30</v>
+      </c>
+      <c r="H68" t="s">
+        <v>289</v>
+      </c>
+      <c r="I68">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C53" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D53" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="C54" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="D54" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="C55" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="D55" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="C56" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="D56" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="C57" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="D57" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="C58" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="D58" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="C59" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="D59" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="C60" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="D60" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="C61" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="D61" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="C62" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="D62" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="C63" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="D63" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="C64" r:id="rId23" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="D64" r:id="rId24" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="C65" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="D65" r:id="rId26" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
+    <hyperlink ref="C66" r:id="rId27" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
+    <hyperlink ref="D66" r:id="rId28" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
+    <hyperlink ref="D68" r:id="rId29" xr:uid="{631711CD-6EC1-40E5-A6EA-78B440F7A08F}"/>
+    <hyperlink ref="D67" r:id="rId30" xr:uid="{43AD2E89-54F8-4CA6-BCA8-D106D3AB64EF}"/>
+    <hyperlink ref="C67" r:id="rId31" xr:uid="{1E842B65-9A4C-41C9-9C6F-DB12418191B3}"/>
+    <hyperlink ref="C68" r:id="rId32" xr:uid="{9C7BDFDE-88D1-4974-AC4A-69730F6164B1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK40"/>
   <sheetViews>
@@ -5852,564 +6412,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I68"/>
-  <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A52" sqref="A52"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="1025" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>232</v>
-      </c>
-      <c r="B53" t="s">
-        <v>195</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E53" t="s">
-        <v>235</v>
-      </c>
-      <c r="G53" t="s">
-        <v>10</v>
-      </c>
-      <c r="H53" t="s">
-        <v>236</v>
-      </c>
-      <c r="I53">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>237</v>
-      </c>
-      <c r="B54" t="s">
-        <v>195</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E54" t="s">
-        <v>239</v>
-      </c>
-      <c r="G54" t="s">
-        <v>10</v>
-      </c>
-      <c r="H54" t="s">
-        <v>236</v>
-      </c>
-      <c r="I54">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>240</v>
-      </c>
-      <c r="B55" t="s">
-        <v>241</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E55" t="s">
-        <v>239</v>
-      </c>
-      <c r="F55" t="s">
-        <v>243</v>
-      </c>
-      <c r="G55" t="s">
-        <v>10</v>
-      </c>
-      <c r="H55" t="s">
-        <v>236</v>
-      </c>
-      <c r="I55">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>244</v>
-      </c>
-      <c r="B56" t="s">
-        <v>245</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E56" t="s">
-        <v>239</v>
-      </c>
-      <c r="F56" t="s">
-        <v>247</v>
-      </c>
-      <c r="G56" t="s">
-        <v>10</v>
-      </c>
-      <c r="H56" t="s">
-        <v>236</v>
-      </c>
-      <c r="I56">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>248</v>
-      </c>
-      <c r="B57" t="s">
-        <v>249</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E57" t="s">
-        <v>235</v>
-      </c>
-      <c r="F57" t="s">
-        <v>251</v>
-      </c>
-      <c r="G57" t="s">
-        <v>10</v>
-      </c>
-      <c r="H57" t="s">
-        <v>236</v>
-      </c>
-      <c r="I57">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>252</v>
-      </c>
-      <c r="B58" t="s">
-        <v>159</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E58" t="s">
-        <v>239</v>
-      </c>
-      <c r="F58" t="s">
-        <v>254</v>
-      </c>
-      <c r="G58" t="s">
-        <v>10</v>
-      </c>
-      <c r="H58" t="s">
-        <v>236</v>
-      </c>
-      <c r="I58">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>255</v>
-      </c>
-      <c r="B59" t="s">
-        <v>159</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E59" t="s">
-        <v>235</v>
-      </c>
-      <c r="F59" t="s">
-        <v>254</v>
-      </c>
-      <c r="G59" t="s">
-        <v>10</v>
-      </c>
-      <c r="H59" t="s">
-        <v>236</v>
-      </c>
-      <c r="I59">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>257</v>
-      </c>
-      <c r="B60" t="s">
-        <v>159</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E60" t="s">
-        <v>235</v>
-      </c>
-      <c r="F60" t="s">
-        <v>259</v>
-      </c>
-      <c r="G60" t="s">
-        <v>10</v>
-      </c>
-      <c r="H60" t="s">
-        <v>236</v>
-      </c>
-      <c r="I60">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>260</v>
-      </c>
-      <c r="B61" t="s">
-        <v>159</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E61" t="s">
-        <v>239</v>
-      </c>
-      <c r="F61" t="s">
-        <v>259</v>
-      </c>
-      <c r="G61" t="s">
-        <v>10</v>
-      </c>
-      <c r="H61" t="s">
-        <v>236</v>
-      </c>
-      <c r="I61">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>262</v>
-      </c>
-      <c r="B62" t="s">
-        <v>159</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E62" t="s">
-        <v>239</v>
-      </c>
-      <c r="F62" t="s">
-        <v>264</v>
-      </c>
-      <c r="G62" t="s">
-        <v>10</v>
-      </c>
-      <c r="H62" t="s">
-        <v>236</v>
-      </c>
-      <c r="I62">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>265</v>
-      </c>
-      <c r="B63" t="s">
-        <v>159</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E63" t="s">
-        <v>235</v>
-      </c>
-      <c r="F63" t="s">
-        <v>264</v>
-      </c>
-      <c r="G63" t="s">
-        <v>10</v>
-      </c>
-      <c r="H63" t="s">
-        <v>236</v>
-      </c>
-      <c r="I63">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>267</v>
-      </c>
-      <c r="B64" t="s">
-        <v>268</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E64" t="s">
-        <v>235</v>
-      </c>
-      <c r="F64" t="s">
-        <v>270</v>
-      </c>
-      <c r="G64" t="s">
-        <v>10</v>
-      </c>
-      <c r="H64" t="s">
-        <v>236</v>
-      </c>
-      <c r="I64">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>271</v>
-      </c>
-      <c r="B65" t="s">
-        <v>272</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E65" t="s">
-        <v>239</v>
-      </c>
-      <c r="F65" t="s">
-        <v>274</v>
-      </c>
-      <c r="G65" t="s">
-        <v>10</v>
-      </c>
-      <c r="H65" t="s">
-        <v>236</v>
-      </c>
-      <c r="I65">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>13001</v>
-      </c>
-      <c r="B66" t="s">
-        <v>272</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E66" t="s">
-        <v>239</v>
-      </c>
-      <c r="F66" t="s">
-        <v>276</v>
-      </c>
-      <c r="G66" t="s">
-        <v>10</v>
-      </c>
-      <c r="H66" t="s">
-        <v>236</v>
-      </c>
-      <c r="I66">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>430</v>
-      </c>
-      <c r="B67" t="s">
-        <v>431</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="E67" t="s">
-        <v>235</v>
-      </c>
-      <c r="F67" t="s">
-        <v>254</v>
-      </c>
-      <c r="G67" t="s">
-        <v>30</v>
-      </c>
-      <c r="H67" t="s">
-        <v>289</v>
-      </c>
-      <c r="I67">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>432</v>
-      </c>
-      <c r="B68" t="s">
-        <v>431</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="E68" t="s">
-        <v>239</v>
-      </c>
-      <c r="F68" t="s">
-        <v>254</v>
-      </c>
-      <c r="G68" t="s">
-        <v>30</v>
-      </c>
-      <c r="H68" t="s">
-        <v>289</v>
-      </c>
-      <c r="I68">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C53" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="D53" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="C54" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="D54" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="C55" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="D55" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="C56" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="D56" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="C57" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="D57" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="C58" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="D58" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
-    <hyperlink ref="C59" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
-    <hyperlink ref="D59" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
-    <hyperlink ref="C60" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
-    <hyperlink ref="D60" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
-    <hyperlink ref="C61" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
-    <hyperlink ref="D61" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
-    <hyperlink ref="C62" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
-    <hyperlink ref="D62" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
-    <hyperlink ref="C63" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
-    <hyperlink ref="D63" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
-    <hyperlink ref="C64" r:id="rId23" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
-    <hyperlink ref="D64" r:id="rId24" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
-    <hyperlink ref="C65" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
-    <hyperlink ref="D65" r:id="rId26" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
-    <hyperlink ref="C66" r:id="rId27" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
-    <hyperlink ref="D66" r:id="rId28" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
-    <hyperlink ref="D68" r:id="rId29" xr:uid="{631711CD-6EC1-40E5-A6EA-78B440F7A08F}"/>
-    <hyperlink ref="D67" r:id="rId30" xr:uid="{43AD2E89-54F8-4CA6-BCA8-D106D3AB64EF}"/>
-    <hyperlink ref="C67" r:id="rId31" xr:uid="{1E842B65-9A4C-41C9-9C6F-DB12418191B3}"/>
-    <hyperlink ref="C68" r:id="rId32" xr:uid="{9C7BDFDE-88D1-4974-AC4A-69730F6164B1}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6453,7 +6461,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="13" t="s">
         <v>281</v>
       </c>
       <c r="B2" t="s">
@@ -6476,7 +6484,7 @@
         <v>287</v>
       </c>
       <c r="I2" t="s">
-        <v>288</v>
+        <v>135</v>
       </c>
       <c r="J2" t="s">
         <v>289</v>
@@ -6549,7 +6557,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="13" t="s">
         <v>301</v>
       </c>
       <c r="B5" t="s">
@@ -6627,7 +6635,7 @@
     <hyperlink ref="D6" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>